<commit_message>
investment and speculative revenue are separated
</commit_message>
<xml_diff>
--- a/stat.xlsx
+++ b/stat.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="26">
   <si>
     <t xml:space="preserve">date</t>
   </si>
@@ -31,7 +31,52 @@
     <t xml:space="preserve">balance</t>
   </si>
   <si>
-    <t xml:space="preserve">profit</t>
+    <t xml:space="preserve">irr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">revenue_s</t>
+  </si>
+  <si>
+    <t xml:space="preserve">apy1_s</t>
+  </si>
+  <si>
+    <t xml:space="preserve">apy7_s</t>
+  </si>
+  <si>
+    <t xml:space="preserve">apy30_s</t>
+  </si>
+  <si>
+    <t xml:space="preserve">apy91_s</t>
+  </si>
+  <si>
+    <t xml:space="preserve">apyAll_s</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cpy_s</t>
+  </si>
+  <si>
+    <t xml:space="preserve">revenue_i</t>
+  </si>
+  <si>
+    <t xml:space="preserve">apy1_i</t>
+  </si>
+  <si>
+    <t xml:space="preserve">apy7_i</t>
+  </si>
+  <si>
+    <t xml:space="preserve">apy30_i</t>
+  </si>
+  <si>
+    <t xml:space="preserve">apy91_i</t>
+  </si>
+  <si>
+    <t xml:space="preserve">apyAll_i</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cpy_i</t>
+  </si>
+  <si>
+    <t xml:space="preserve">revenue</t>
   </si>
   <si>
     <t xml:space="preserve">apy1</t>
@@ -49,9 +94,6 @@
     <t xml:space="preserve">apyAll</t>
   </si>
   <si>
-    <t xml:space="preserve">irr</t>
-  </si>
-  <si>
     <t xml:space="preserve">cpy</t>
   </si>
   <si>
@@ -66,7 +108,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -87,6 +129,13 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -141,11 +190,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -168,12 +217,12 @@
       <rgbColor rgb="FFFFFF00"/>
       <rgbColor rgb="FFFF00FF"/>
       <rgbColor rgb="FF00FFFF"/>
-      <rgbColor rgb="FF7E0021"/>
+      <rgbColor rgb="FF800000"/>
       <rgbColor rgb="FF008000"/>
       <rgbColor rgb="FF000080"/>
       <rgbColor rgb="FF808000"/>
-      <rgbColor rgb="FFBF0041"/>
-      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF158466"/>
       <rgbColor rgb="FFB3B3B3"/>
       <rgbColor rgb="FF808080"/>
       <rgbColor rgb="FF9999FF"/>
@@ -182,7 +231,7 @@
       <rgbColor rgb="FFCCFFFF"/>
       <rgbColor rgb="FF660066"/>
       <rgbColor rgb="FFFF8080"/>
-      <rgbColor rgb="FF0066CC"/>
+      <rgbColor rgb="FF2A6099"/>
       <rgbColor rgb="FFDDDDDD"/>
       <rgbColor rgb="FF000080"/>
       <rgbColor rgb="FFFF00FF"/>
@@ -196,7 +245,7 @@
       <rgbColor rgb="FFCCFFFF"/>
       <rgbColor rgb="FFCCFFCC"/>
       <rgbColor rgb="FFFFFF99"/>
-      <rgbColor rgb="FF83CAFF"/>
+      <rgbColor rgb="FF99CCFF"/>
       <rgbColor rgb="FFFF99CC"/>
       <rgbColor rgb="FFCC99FF"/>
       <rgbColor rgb="FFFFCC99"/>
@@ -205,7 +254,7 @@
       <rgbColor rgb="FF99CC00"/>
       <rgbColor rgb="FFFFCC00"/>
       <rgbColor rgb="FFFF9900"/>
-      <rgbColor rgb="FFFF420E"/>
+      <rgbColor rgb="FFFF6600"/>
       <rgbColor rgb="FF666699"/>
       <rgbColor rgb="FF969696"/>
       <rgbColor rgb="FF004586"/>
@@ -221,7 +270,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -276,7 +325,6 @@
                 </a:pPr>
               </a:p>
             </c:txPr>
-            <c:dLblPos val="r"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -311,12 +359,6 @@
                 <c:pt idx="4">
                   <c:v>45188</c:v>
                 </c:pt>
-                <c:pt idx="5">
-                  <c:v>45189</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>45190</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -341,22 +383,16 @@
                 <c:pt idx="4">
                   <c:v>5000</c:v>
                 </c:pt>
-                <c:pt idx="5">
-                  <c:v>5000</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>5000</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="72412712"/>
-        <c:axId val="81721581"/>
+        <c:axId val="46285443"/>
+        <c:axId val="56916727"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="72412712"/>
+        <c:axId val="46285443"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -371,7 +407,16 @@
             </a:ln>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="yyyy\-mm\-dd" sourceLinked="1"/>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln w="0">
+              <a:solidFill>
+                <a:srgbClr val="dddddd"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -393,12 +438,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="81721581"/>
+        <c:crossAx val="56916727"/>
         <c:crossesAt val="0"/>
-        <c:crossBetween val="midCat"/>
+        <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="81721581"/>
+        <c:axId val="56916727"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -413,7 +458,7 @@
             </a:ln>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -435,9 +480,9 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="72412712"/>
+        <c:crossAx val="46285443"/>
         <c:crossesAt val="0"/>
-        <c:crossBetween val="midCat"/>
+        <c:crossBetween val="between"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -483,7 +528,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -498,22 +543,22 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$E$1</c:f>
+              <c:f>Sheet1!$K$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>apy1</c:v>
+                  <c:v>cpy_s</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:srgbClr val="004586"/>
+              <a:srgbClr val="158466"/>
             </a:solidFill>
             <a:ln w="0">
               <a:solidFill>
-                <a:srgbClr val="004586"/>
+                <a:srgbClr val="158466"/>
               </a:solidFill>
             </a:ln>
           </c:spPr>
@@ -522,7 +567,7 @@
             <c:size val="2"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="004586"/>
+                <a:srgbClr val="158466"/>
               </a:solidFill>
             </c:spPr>
           </c:marker>
@@ -538,7 +583,6 @@
                 </a:pPr>
               </a:p>
             </c:txPr>
-            <c:dLblPos val="r"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -554,10 +598,10 @@
           </c:dLbls>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$1000</c:f>
+              <c:f>Sheet1!$A$2:$A$10000</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="999"/>
+                <c:ptCount val="9999"/>
                 <c:pt idx="0">
                   <c:v>45184</c:v>
                 </c:pt>
@@ -572,22 +616,16 @@
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>45188</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>45189</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>45190</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$E$2:$E$1000</c:f>
+              <c:f>Sheet1!$K$2:$K$10000</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="999"/>
+                <c:ptCount val="9999"/>
                 <c:pt idx="1">
                   <c:v>0</c:v>
                 </c:pt>
@@ -598,12 +636,6 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="6">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -616,22 +648,22 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$F$1</c:f>
+              <c:f>Sheet1!$R$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>apy7</c:v>
+                  <c:v>cpy_i</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:srgbClr val="ff420e"/>
+              <a:srgbClr val="800080"/>
             </a:solidFill>
             <a:ln w="0">
               <a:solidFill>
-                <a:srgbClr val="ff420e"/>
+                <a:srgbClr val="800080"/>
               </a:solidFill>
             </a:ln>
           </c:spPr>
@@ -640,7 +672,7 @@
             <c:size val="2"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="ff420e"/>
+                <a:srgbClr val="800080"/>
               </a:solidFill>
             </c:spPr>
           </c:marker>
@@ -656,7 +688,6 @@
                 </a:pPr>
               </a:p>
             </c:txPr>
-            <c:dLblPos val="r"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -672,10 +703,10 @@
           </c:dLbls>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$1000</c:f>
+              <c:f>Sheet1!$A$2:$A$10000</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="999"/>
+                <c:ptCount val="9999"/>
                 <c:pt idx="0">
                   <c:v>45184</c:v>
                 </c:pt>
@@ -690,23 +721,26 @@
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>45188</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>45189</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>45190</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$F$2:$F$1000</c:f>
+              <c:f>Sheet1!$R$2:$R$10000</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="999"/>
-                <c:pt idx="6">
+                <c:ptCount val="9999"/>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -719,24 +753,23 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$G$1</c:f>
+              <c:f>Sheet1!$Y$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>apy30</c:v>
+                  <c:v>cpy</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:srgbClr val="bf0041"/>
+              <a:srgbClr val="2a6099"/>
             </a:solidFill>
-            <a:ln w="18360">
-              <a:solidFill>
-                <a:srgbClr val="bf0041"/>
-              </a:solidFill>
-              <a:round/>
+            <a:ln w="0">
+              <a:solidFill>
+                <a:srgbClr val="2a6099"/>
+              </a:solidFill>
             </a:ln>
           </c:spPr>
           <c:marker>
@@ -744,7 +777,7 @@
             <c:size val="2"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="bf0041"/>
+                <a:srgbClr val="2a6099"/>
               </a:solidFill>
             </c:spPr>
           </c:marker>
@@ -760,7 +793,6 @@
                 </a:pPr>
               </a:p>
             </c:txPr>
-            <c:dLblPos val="r"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -776,10 +808,10 @@
           </c:dLbls>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$1000</c:f>
+              <c:f>Sheet1!$A$2:$A$10000</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="999"/>
+                <c:ptCount val="9999"/>
                 <c:pt idx="0">
                   <c:v>45184</c:v>
                 </c:pt>
@@ -794,369 +826,38 @@
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>45188</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>45189</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>45190</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$G$2:$G$1000</c:f>
+              <c:f>Sheet1!$Y$2:$Y$10000</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="999"/>
+                <c:ptCount val="9999"/>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:ser>
-          <c:idx val="3"/>
-          <c:order val="3"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$H$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>apy91</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="ff0000"/>
-            </a:solidFill>
-            <a:ln w="36720">
-              <a:solidFill>
-                <a:srgbClr val="ff0000"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="triangle"/>
-            <c:size val="2"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="ff0000"/>
-              </a:solidFill>
-            </c:spPr>
-          </c:marker>
-          <c:dLbls>
-            <c:txPr>
-              <a:bodyPr wrap="none"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-                    <a:latin typeface="Arial"/>
-                  </a:defRPr>
-                </a:pPr>
-              </a:p>
-            </c:txPr>
-            <c:dLblPos val="r"/>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="0"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:separator> </c:separator>
-            <c:showLeaderLines val="1"/>
-            <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:showLeaderLines val="1"/>
-              </c:ext>
-            </c:extLst>
-          </c:dLbls>
-          <c:xVal>
-            <c:numRef>
-              <c:f>Sheet1!$A$2:$A$1000</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="999"/>
-                <c:pt idx="0">
-                  <c:v>45184</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>45185</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>45186</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>45187</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>45188</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>45189</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>45190</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Sheet1!$H$2:$H$1000</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="999"/>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:ser>
-          <c:idx val="4"/>
-          <c:order val="4"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$I$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>apyAll</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="7e0021"/>
-            </a:solidFill>
-            <a:ln w="0">
-              <a:solidFill>
-                <a:srgbClr val="7e0021"/>
-              </a:solidFill>
-            </a:ln>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="triangle"/>
-            <c:size val="2"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="7e0021"/>
-              </a:solidFill>
-            </c:spPr>
-          </c:marker>
-          <c:dLbls>
-            <c:txPr>
-              <a:bodyPr wrap="none"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-                    <a:latin typeface="Arial"/>
-                  </a:defRPr>
-                </a:pPr>
-              </a:p>
-            </c:txPr>
-            <c:dLblPos val="r"/>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="0"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:separator> </c:separator>
-            <c:showLeaderLines val="1"/>
-            <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:showLeaderLines val="1"/>
-              </c:ext>
-            </c:extLst>
-          </c:dLbls>
-          <c:xVal>
-            <c:numRef>
-              <c:f>Sheet1!$A$2:$A$1000</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="999"/>
-                <c:pt idx="0">
-                  <c:v>45184</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>45185</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>45186</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>45187</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>45188</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>45189</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>45190</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Sheet1!$I$2:$I$1000</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="999"/>
-                <c:pt idx="1">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:ser>
-          <c:idx val="5"/>
-          <c:order val="5"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$J$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>irr</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="83caff"/>
-            </a:solidFill>
-            <a:ln w="0">
-              <a:solidFill>
-                <a:srgbClr val="83caff"/>
-              </a:solidFill>
-            </a:ln>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="triangle"/>
-            <c:size val="2"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="83caff"/>
-              </a:solidFill>
-            </c:spPr>
-          </c:marker>
-          <c:dLbls>
-            <c:txPr>
-              <a:bodyPr wrap="none"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-                    <a:latin typeface="Arial"/>
-                  </a:defRPr>
-                </a:pPr>
-              </a:p>
-            </c:txPr>
-            <c:dLblPos val="r"/>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="0"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:separator> </c:separator>
-            <c:showLeaderLines val="1"/>
-            <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:showLeaderLines val="1"/>
-              </c:ext>
-            </c:extLst>
-          </c:dLbls>
-          <c:xVal>
-            <c:numRef>
-              <c:f>Sheet1!$A$2:$A$1000</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="999"/>
-                <c:pt idx="0">
-                  <c:v>45184</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>45185</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>45186</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>45187</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>45188</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>45189</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>45190</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Sheet1!$J$2:$J$1000</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="999"/>
-                <c:pt idx="1">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:axId val="90102523"/>
-        <c:axId val="55357842"/>
+        <c:axId val="95212988"/>
+        <c:axId val="25754079"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="90102523"/>
+        <c:axId val="95212988"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1171,6 +872,15 @@
             </a:ln>
           </c:spPr>
         </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln w="0">
+              <a:solidFill>
+                <a:srgbClr val="dddddd"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:minorGridlines>
         <c:numFmt formatCode="yyyy\-mm\-dd" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
@@ -1193,16 +903,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="55357842"/>
+        <c:crossAx val="25754079"/>
         <c:crossesAt val="0"/>
-        <c:crossBetween val="midCat"/>
+        <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="55357842"/>
+        <c:axId val="25754079"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="80"/>
-          <c:min val="-10"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -1215,16 +923,7 @@
             </a:ln>
           </c:spPr>
         </c:majorGridlines>
-        <c:minorGridlines>
-          <c:spPr>
-            <a:ln w="0">
-              <a:solidFill>
-                <a:srgbClr val="dddddd"/>
-              </a:solidFill>
-            </a:ln>
-          </c:spPr>
-        </c:minorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1246,10 +945,9 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="90102523"/>
+        <c:crossAx val="95212988"/>
         <c:crossesAt val="0"/>
-        <c:crossBetween val="midCat"/>
-        <c:majorUnit val="10"/>
+        <c:crossBetween val="between"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -1295,7 +993,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1310,22 +1008,22 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$K$1</c:f>
+              <c:f>Sheet1!$G$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>cpy</c:v>
+                  <c:v>apy7_s</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:srgbClr val="004586"/>
+              <a:srgbClr val="158466"/>
             </a:solidFill>
             <a:ln w="0">
               <a:solidFill>
-                <a:srgbClr val="004586"/>
+                <a:srgbClr val="158466"/>
               </a:solidFill>
             </a:ln>
           </c:spPr>
@@ -1334,7 +1032,7 @@
             <c:size val="2"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="004586"/>
+                <a:srgbClr val="158466"/>
               </a:solidFill>
             </c:spPr>
           </c:marker>
@@ -1350,7 +1048,6 @@
                 </a:pPr>
               </a:p>
             </c:txPr>
-            <c:dLblPos val="r"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -1366,10 +1063,10 @@
           </c:dLbls>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$1000</c:f>
+              <c:f>Sheet1!$A$2:$A$10000</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="999"/>
+                <c:ptCount val="9999"/>
                 <c:pt idx="0">
                   <c:v>45184</c:v>
                 </c:pt>
@@ -1384,50 +1081,212 @@
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>45188</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>45189</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>45190</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$K$2:$K$1000</c:f>
+              <c:f>Sheet1!$G$2:$G$10000</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="999"/>
-                <c:pt idx="1">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0</c:v>
-                </c:pt>
+                <c:ptCount val="9999"/>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="43206598"/>
-        <c:axId val="73376826"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$N$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>apy7_i</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="800080"/>
+            </a:solidFill>
+            <a:ln w="0">
+              <a:solidFill>
+                <a:srgbClr val="800080"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="diamond"/>
+            <c:size val="2"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="800080"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:txPr>
+              <a:bodyPr wrap="none"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:separator> </c:separator>
+            <c:showLeaderLines val="1"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$2:$A$10000</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9999"/>
+                <c:pt idx="0">
+                  <c:v>45184</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>45185</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>45186</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>45187</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>45188</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$N$2:$N$10000</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9999"/>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$U$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>apy7</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="2a6099"/>
+            </a:solidFill>
+            <a:ln w="0">
+              <a:solidFill>
+                <a:srgbClr val="2a6099"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="triangle"/>
+            <c:size val="2"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="2a6099"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:txPr>
+              <a:bodyPr wrap="none"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:separator> </c:separator>
+            <c:showLeaderLines val="1"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$2:$A$10000</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9999"/>
+                <c:pt idx="0">
+                  <c:v>45184</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>45185</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>45186</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>45187</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>45188</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$U$2:$U$10000</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9999"/>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:axId val="55216033"/>
+        <c:axId val="1745725"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="43206598"/>
+        <c:axId val="55216033"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1442,6 +1301,15 @@
             </a:ln>
           </c:spPr>
         </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln w="0">
+              <a:solidFill>
+                <a:srgbClr val="dddddd"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:minorGridlines>
         <c:numFmt formatCode="yyyy\-mm\-dd" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
@@ -1464,12 +1332,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="73376826"/>
+        <c:crossAx val="1745725"/>
         <c:crossesAt val="0"/>
-        <c:crossBetween val="midCat"/>
+        <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="73376826"/>
+        <c:axId val="1745725"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1484,7 +1352,7 @@
             </a:ln>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1506,9 +1374,579 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="43206598"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
+        <c:crossAx val="55216033"/>
+        <c:crossesAt val="0"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="0">
+          <a:solidFill>
+            <a:srgbClr val="b3b3b3"/>
+          </a:solidFill>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="0">
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+              <a:latin typeface="Arial"/>
+            </a:defRPr>
+          </a:pPr>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="span"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:srgbClr val="ffffff"/>
+    </a:solidFill>
+    <a:ln w="0">
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$J$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>apyAll_s</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="158466"/>
+            </a:solidFill>
+            <a:ln w="0">
+              <a:solidFill>
+                <a:srgbClr val="158466"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="diamond"/>
+            <c:size val="2"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="158466"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:txPr>
+              <a:bodyPr wrap="none"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:separator> </c:separator>
+            <c:showLeaderLines val="1"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$2:$A$10000</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9999"/>
+                <c:pt idx="0">
+                  <c:v>45184</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>45185</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>45186</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>45187</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>45188</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$J$2:$J$10000</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9999"/>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$Q$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>apyAll_i</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="800080"/>
+            </a:solidFill>
+            <a:ln w="0">
+              <a:solidFill>
+                <a:srgbClr val="800080"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="triangle"/>
+            <c:size val="2"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="800080"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:txPr>
+              <a:bodyPr wrap="none"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:separator> </c:separator>
+            <c:showLeaderLines val="1"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$2:$A$10000</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9999"/>
+                <c:pt idx="0">
+                  <c:v>45184</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>45185</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>45186</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>45187</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>45188</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$Q$2:$Q$10000</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9999"/>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$X$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>apyAll</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="2a6099"/>
+            </a:solidFill>
+            <a:ln w="0">
+              <a:solidFill>
+                <a:srgbClr val="2a6099"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="triangle"/>
+            <c:size val="2"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="2a6099"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:txPr>
+              <a:bodyPr wrap="none"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:separator> </c:separator>
+            <c:showLeaderLines val="1"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$2:$A$10000</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9999"/>
+                <c:pt idx="0">
+                  <c:v>45184</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>45185</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>45186</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>45187</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>45188</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$X$2:$X$10000</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9999"/>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>irr</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="004586"/>
+            </a:solidFill>
+            <a:ln w="0">
+              <a:solidFill>
+                <a:srgbClr val="004586"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="square"/>
+            <c:size val="2"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="004586"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:txPr>
+              <a:bodyPr wrap="none"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:separator> </c:separator>
+            <c:showLeaderLines val="1"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$2:$A$10000</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9999"/>
+                <c:pt idx="0">
+                  <c:v>45184</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>45185</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>45186</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>45187</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>45188</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$D$2:$D$10000</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9999"/>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:axId val="9364347"/>
+        <c:axId val="22408476"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="9364347"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="0">
+              <a:solidFill>
+                <a:srgbClr val="b3b3b3"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln w="0">
+              <a:solidFill>
+                <a:srgbClr val="dddddd"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:numFmt formatCode="yyyy\-mm\-dd" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="0">
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="22408476"/>
+        <c:crossesAt val="0"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="22408476"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="0">
+              <a:solidFill>
+                <a:srgbClr val="b3b3b3"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="0">
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="9364347"/>
+        <c:crossesAt val="0"/>
+        <c:crossBetween val="between"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -1559,15 +1997,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>349560</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>28800</xdr:rowOff>
+      <xdr:colOff>330840</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>142200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>398520</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>69480</xdr:rowOff>
+      <xdr:colOff>432360</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>121680</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1575,8 +2013,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="349560" y="678960"/>
-        <a:ext cx="8177040" cy="1503720"/>
+        <a:off x="330840" y="467280"/>
+        <a:ext cx="8229600" cy="2743200"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1588,16 +2026,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>345240</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>129240</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>604440</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>55080</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>196200</xdr:colOff>
-      <xdr:row>40</xdr:row>
-      <xdr:rowOff>153000</xdr:rowOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>705960</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>34560</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1605,8 +2043,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="345240" y="2405160"/>
-        <a:ext cx="16919640" cy="4250160"/>
+        <a:off x="8732520" y="380160"/>
+        <a:ext cx="8229600" cy="2743200"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1618,16 +2056,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>722520</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>330120</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>64080</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>771480</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>40680</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>431640</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>43920</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1635,12 +2073,42 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="8850600" y="650160"/>
-        <a:ext cx="8177040" cy="1503720"/>
+        <a:off x="330120" y="3477960"/>
+        <a:ext cx="8229600" cy="2743200"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>694080</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>99000</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>795600</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>78840</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame>
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name=""/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="8822160" y="3512880"/>
+        <a:ext cx="8229600" cy="2743200"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1654,7 +2122,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K42"/>
+  <dimension ref="A1:Y102"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
@@ -1663,7 +2131,7 @@
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
@@ -1696,9 +2164,51 @@
       <c r="K1" s="0" t="s">
         <v>10</v>
       </c>
+      <c r="L1" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="U1" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="V1" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="W1" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="X1" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y1" s="0" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="n">
+      <c r="A2" s="2" t="n">
         <v>45184</v>
       </c>
       <c r="B2" s="0" t="n">
@@ -1707,33 +2217,75 @@
       <c r="C2" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="D2" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>11</v>
+      <c r="D2" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="E2" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="G2" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="H2" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="I2" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="J2" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="K2" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="L2" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="M2" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="N2" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="O2" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="P2" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q2" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="R2" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="S2" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="T2" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="U2" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="V2" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="W2" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="X2" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="Y2" s="0" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="n">
+      <c r="A3" s="2" t="n">
         <v>45185</v>
       </c>
       <c r="B3" s="0" t="n">
@@ -1748,17 +2300,17 @@
       <c r="E3" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="F3" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="I3" s="0" t="n">
-        <v>0</v>
+      <c r="F3" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G3" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="H3" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="I3" s="0" t="s">
+        <v>25</v>
       </c>
       <c r="J3" s="0" t="n">
         <v>0</v>
@@ -1766,9 +2318,51 @@
       <c r="K3" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="L3" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="M3" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="N3" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="O3" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="P3" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q3" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="R3" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="S3" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="T3" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="U3" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="V3" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="W3" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="X3" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y3" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="n">
+      <c r="A4" s="2" t="n">
         <v>45186</v>
       </c>
       <c r="B4" s="0" t="n">
@@ -1783,17 +2377,17 @@
       <c r="E4" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="F4" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="I4" s="0" t="n">
-        <v>0</v>
+      <c r="F4" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G4" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="H4" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="I4" s="0" t="s">
+        <v>25</v>
       </c>
       <c r="J4" s="0" t="n">
         <v>0</v>
@@ -1801,9 +2395,51 @@
       <c r="K4" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="L4" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="M4" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="N4" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="O4" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="P4" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q4" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="R4" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="S4" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="T4" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="U4" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="V4" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="W4" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="X4" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y4" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="n">
+      <c r="A5" s="2" t="n">
         <v>45187</v>
       </c>
       <c r="B5" s="0" t="n">
@@ -1818,17 +2454,17 @@
       <c r="E5" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="F5" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="I5" s="0" t="n">
-        <v>0</v>
+      <c r="F5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G5" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="H5" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="I5" s="0" t="s">
+        <v>25</v>
       </c>
       <c r="J5" s="0" t="n">
         <v>0</v>
@@ -1836,9 +2472,51 @@
       <c r="K5" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="L5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="M5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="N5" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="O5" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="P5" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="R5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="S5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="T5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="U5" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="V5" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="W5" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="X5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y5" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="n">
+      <c r="A6" s="2" t="n">
         <v>45188</v>
       </c>
       <c r="B6" s="0" t="n">
@@ -1853,17 +2531,17 @@
       <c r="E6" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="F6" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="H6" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="I6" s="0" t="n">
-        <v>0</v>
+      <c r="F6" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G6" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="H6" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="I6" s="0" t="s">
+        <v>25</v>
       </c>
       <c r="J6" s="0" t="n">
         <v>0</v>
@@ -1871,178 +2549,336 @@
       <c r="K6" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="L6" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="M6" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="N6" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="O6" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="P6" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q6" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="R6" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="S6" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="T6" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="U6" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="V6" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="W6" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="X6" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y6" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="n">
-        <v>45189</v>
-      </c>
-      <c r="B7" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="C7" s="0" t="n">
-        <v>5000</v>
-      </c>
-      <c r="D7" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E7" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="F7" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="G7" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="H7" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="I7" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="J7" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="K7" s="0" t="n">
-        <v>0</v>
-      </c>
+      <c r="A7" s="2"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="1" t="n">
-        <v>45190</v>
-      </c>
-      <c r="B8" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="C8" s="0" t="n">
-        <v>5000</v>
-      </c>
-      <c r="D8" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E8" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="F8" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="G8" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="H8" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="I8" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="J8" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="K8" s="0" t="n">
-        <v>0</v>
-      </c>
+      <c r="A8" s="2"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="1"/>
+      <c r="A9" s="2"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="1"/>
+      <c r="A10" s="2"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="1"/>
+      <c r="A11" s="2"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="1"/>
+      <c r="A12" s="2"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="1"/>
+      <c r="A13" s="2"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="1"/>
+      <c r="A14" s="2"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="1"/>
+      <c r="A15" s="2"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="1"/>
+      <c r="A16" s="2"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="1"/>
+      <c r="A17" s="2"/>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="1"/>
+      <c r="A18" s="2"/>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="1"/>
+      <c r="A19" s="2"/>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="1"/>
+      <c r="A20" s="2"/>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="1"/>
+      <c r="A21" s="2"/>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="1"/>
+      <c r="A22" s="2"/>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="1"/>
+      <c r="A23" s="2"/>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="1"/>
+      <c r="A24" s="2"/>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="1"/>
+      <c r="A25" s="2"/>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="1"/>
+      <c r="A26" s="2"/>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="1"/>
+      <c r="A27" s="2"/>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="1"/>
+      <c r="A28" s="2"/>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="1"/>
+      <c r="A29" s="2"/>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="1"/>
+      <c r="A30" s="2"/>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="1"/>
+      <c r="A31" s="2"/>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="1"/>
+      <c r="A32" s="2"/>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="1"/>
+      <c r="A33" s="2"/>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="1"/>
+      <c r="A34" s="2"/>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="1"/>
+      <c r="A35" s="2"/>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="1"/>
+      <c r="A36" s="2"/>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="1"/>
+      <c r="A37" s="2"/>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="1"/>
+      <c r="A38" s="2"/>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="1"/>
+      <c r="A39" s="2"/>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="1"/>
+      <c r="A40" s="2"/>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="1"/>
+      <c r="A41" s="2"/>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="1"/>
+      <c r="A42" s="2"/>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="2"/>
+    </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="2"/>
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="2"/>
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="2"/>
+    </row>
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="2"/>
+    </row>
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="2"/>
+    </row>
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="2"/>
+    </row>
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="2"/>
+    </row>
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="2"/>
+    </row>
+    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="2"/>
+    </row>
+    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="2"/>
+    </row>
+    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="2"/>
+    </row>
+    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="2"/>
+    </row>
+    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="2"/>
+    </row>
+    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="2"/>
+    </row>
+    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="2"/>
+    </row>
+    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="2"/>
+    </row>
+    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="2"/>
+    </row>
+    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="2"/>
+    </row>
+    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="2"/>
+    </row>
+    <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A63" s="2"/>
+    </row>
+    <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A64" s="2"/>
+    </row>
+    <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A65" s="2"/>
+    </row>
+    <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A66" s="2"/>
+    </row>
+    <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A67" s="2"/>
+    </row>
+    <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A68" s="2"/>
+    </row>
+    <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A69" s="2"/>
+    </row>
+    <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A70" s="2"/>
+    </row>
+    <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A71" s="2"/>
+    </row>
+    <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A72" s="2"/>
+    </row>
+    <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A73" s="2"/>
+    </row>
+    <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A74" s="2"/>
+    </row>
+    <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A75" s="2"/>
+    </row>
+    <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A76" s="2"/>
+    </row>
+    <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A77" s="2"/>
+    </row>
+    <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A78" s="2"/>
+    </row>
+    <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A79" s="2"/>
+    </row>
+    <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A80" s="2"/>
+    </row>
+    <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A81" s="2"/>
+    </row>
+    <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A82" s="2"/>
+    </row>
+    <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A83" s="2"/>
+    </row>
+    <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A84" s="2"/>
+    </row>
+    <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A85" s="2"/>
+    </row>
+    <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A86" s="2"/>
+    </row>
+    <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A87" s="2"/>
+    </row>
+    <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A88" s="2"/>
+    </row>
+    <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A89" s="2"/>
+    </row>
+    <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A90" s="2"/>
+    </row>
+    <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A91" s="2"/>
+    </row>
+    <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A92" s="2"/>
+    </row>
+    <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A93" s="2"/>
+    </row>
+    <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A94" s="2"/>
+    </row>
+    <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A95" s="2"/>
+    </row>
+    <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A96" s="2"/>
+    </row>
+    <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A97" s="2"/>
+    </row>
+    <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A98" s="2"/>
+    </row>
+    <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A99" s="2"/>
+    </row>
+    <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A100" s="2"/>
+    </row>
+    <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A101" s="2"/>
+    </row>
+    <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A102" s="2"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
an asset as a part of capital fix time overlaps
</commit_message>
<xml_diff>
--- a/stat.xlsx
+++ b/stat.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="34">
   <si>
     <t xml:space="preserve">date</t>
   </si>
@@ -29,6 +29,9 @@
   </si>
   <si>
     <t xml:space="preserve">balance</t>
+  </si>
+  <si>
+    <t xml:space="preserve">debt</t>
   </si>
   <si>
     <t xml:space="preserve">irr</t>
@@ -49,7 +52,7 @@
     <t xml:space="preserve">apy91</t>
   </si>
   <si>
-    <t xml:space="preserve">apyAll</t>
+    <t xml:space="preserve">apy</t>
   </si>
   <si>
     <t xml:space="preserve">cpy</t>
@@ -70,7 +73,7 @@
     <t xml:space="preserve">apy91_i</t>
   </si>
   <si>
-    <t xml:space="preserve">apyAll_i</t>
+    <t xml:space="preserve">apy_i</t>
   </si>
   <si>
     <t xml:space="preserve">cpy_i</t>
@@ -91,7 +94,7 @@
     <t xml:space="preserve">apy91_s</t>
   </si>
   <si>
-    <t xml:space="preserve">apyAll_s</t>
+    <t xml:space="preserve">apy_s</t>
   </si>
   <si>
     <t xml:space="preserve">cpy_s</t>
@@ -112,7 +115,7 @@
     <t xml:space="preserve">apy91_o</t>
   </si>
   <si>
-    <t xml:space="preserve">apyAll_o</t>
+    <t xml:space="preserve">apy_o</t>
   </si>
   <si>
     <t xml:space="preserve">cpy_o</t>
@@ -295,7 +298,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart108.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -414,11 +417,119 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="46252617"/>
-        <c:axId val="48474401"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>debt</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="158466"/>
+            </a:solidFill>
+            <a:ln w="0">
+              <a:solidFill>
+                <a:srgbClr val="158466"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="diamond"/>
+            <c:size val="2"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="158466"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:txPr>
+              <a:bodyPr wrap="none"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:separator> </c:separator>
+            <c:showLeaderLines val="1"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$2:$A$1000</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="999"/>
+                <c:pt idx="0">
+                  <c:v>45184</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>45185</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>45186</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>45187</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>45188</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$D$2:$D$1000</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="999"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>400</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:axId val="71426385"/>
+        <c:axId val="40110757"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="46252617"/>
+        <c:axId val="71426385"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -442,7 +553,7 @@
             </a:ln>
           </c:spPr>
         </c:minorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:numFmt formatCode="yyyy\-mm\-dd" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -464,12 +575,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="48474401"/>
+        <c:crossAx val="40110757"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="48474401"/>
+        <c:axId val="40110757"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -506,7 +617,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="46252617"/>
+        <c:crossAx val="71426385"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -554,7 +665,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart109.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -569,7 +680,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$K$1</c:f>
+              <c:f>Sheet1!$L$1:$L$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -649,7 +760,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$K$2:$K$10000</c:f>
+              <c:f>Sheet1!$L$2:$L$10000</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9999"/>
@@ -678,7 +789,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$R$1</c:f>
+              <c:f>Sheet1!$S$1:$S$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -758,7 +869,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$R$2:$R$10000</c:f>
+              <c:f>Sheet1!$S$2:$S$10000</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9999"/>
@@ -787,7 +898,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$Y$1</c:f>
+              <c:f>Sheet1!$Z$1:$Z$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -867,7 +978,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$Y$2:$Y$10000</c:f>
+              <c:f>Sheet1!$Z$2:$Z$10000</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9999"/>
@@ -896,7 +1007,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$AF$1</c:f>
+              <c:f>Sheet1!$AG$1:$AG$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -936,6 +1047,7 @@
                 </a:pPr>
               </a:p>
             </c:txPr>
+            <c:dLblPos val="r"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -975,7 +1087,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$AF$2:$AF$10000</c:f>
+              <c:f>Sheet1!$AG$2:$AG$10000</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9999"/>
@@ -999,11 +1111,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="6403673"/>
-        <c:axId val="64903766"/>
+        <c:axId val="48303930"/>
+        <c:axId val="1092808"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="6403673"/>
+        <c:axId val="48303930"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1049,12 +1161,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="64903766"/>
+        <c:crossAx val="1092808"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="64903766"/>
+        <c:axId val="1092808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1091,7 +1203,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="6403673"/>
+        <c:crossAx val="48303930"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1139,7 +1251,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart110.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1154,7 +1266,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$G$1</c:f>
+              <c:f>Sheet1!$H$1:$H$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1234,7 +1346,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$G$2:$G$10000</c:f>
+              <c:f>Sheet1!$H$2:$H$10000</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9999"/>
@@ -1248,7 +1360,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$N$1</c:f>
+              <c:f>Sheet1!$O$1:$O$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1328,7 +1440,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$N$2:$N$10000</c:f>
+              <c:f>Sheet1!$O$2:$O$10000</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9999"/>
@@ -1342,7 +1454,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$U$1</c:f>
+              <c:f>Sheet1!$V$1:$V$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1422,7 +1534,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$U$2:$U$10000</c:f>
+              <c:f>Sheet1!$V$2:$V$10000</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9999"/>
@@ -1436,7 +1548,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$AB$1</c:f>
+              <c:f>Sheet1!$AC$1:$AC$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1476,6 +1588,7 @@
                 </a:pPr>
               </a:p>
             </c:txPr>
+            <c:dLblPos val="r"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -1515,7 +1628,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$AB$2:$AB$10000</c:f>
+              <c:f>Sheet1!$AC$2:$AC$10000</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9999"/>
@@ -1524,11 +1637,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="26870029"/>
-        <c:axId val="63013643"/>
+        <c:axId val="24478412"/>
+        <c:axId val="88100120"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="26870029"/>
+        <c:axId val="24478412"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1574,12 +1687,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="63013643"/>
+        <c:crossAx val="88100120"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="63013643"/>
+        <c:axId val="88100120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1616,7 +1729,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="26870029"/>
+        <c:crossAx val="24478412"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1664,7 +1777,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart19.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart111.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1679,11 +1792,11 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$J$1</c:f>
+              <c:f>Sheet1!$K$1:$K$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>apyAll</c:v>
+                  <c:v>apy</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1759,7 +1872,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$J$2:$J$10000</c:f>
+              <c:f>Sheet1!$K$2:$K$10000</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9999"/>
@@ -1785,11 +1898,11 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$Q$1</c:f>
+              <c:f>Sheet1!$R$1:$R$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>apyAll_i</c:v>
+                  <c:v>apy_i</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1865,7 +1978,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$Q$2:$Q$10000</c:f>
+              <c:f>Sheet1!$R$2:$R$10000</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9999"/>
@@ -1891,11 +2004,11 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$X$1</c:f>
+              <c:f>Sheet1!$Y$1:$Y$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>apyAll_s</c:v>
+                  <c:v>apy_s</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1971,7 +2084,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$X$2:$X$10000</c:f>
+              <c:f>Sheet1!$Y$2:$Y$10000</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9999"/>
@@ -1997,11 +2110,11 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$AE$1</c:f>
+              <c:f>Sheet1!$AF$1:$AF$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>apyAll_o</c:v>
+                  <c:v>apy_o</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2022,111 +2135,6 @@
             <c:spPr>
               <a:solidFill>
                 <a:srgbClr val="808080"/>
-              </a:solidFill>
-            </c:spPr>
-          </c:marker>
-          <c:dLbls>
-            <c:txPr>
-              <a:bodyPr wrap="none"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-                    <a:latin typeface="Arial"/>
-                  </a:defRPr>
-                </a:pPr>
-              </a:p>
-            </c:txPr>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="0"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:separator> </c:separator>
-            <c:showLeaderLines val="1"/>
-            <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:showLeaderLines val="1"/>
-              </c:ext>
-            </c:extLst>
-          </c:dLbls>
-          <c:xVal>
-            <c:numRef>
-              <c:f>Sheet1!$A$2:$A$10000</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9999"/>
-                <c:pt idx="0">
-                  <c:v>45184</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>45185</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>45186</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>45187</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>45188</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Sheet1!$AE$2:$AE$10000</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9999"/>
-                <c:pt idx="1">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:ser>
-          <c:idx val="4"/>
-          <c:order val="4"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$D$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>irr</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="004586"/>
-            </a:solidFill>
-            <a:ln w="0">
-              <a:solidFill>
-                <a:srgbClr val="004586"/>
-              </a:solidFill>
-            </a:ln>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="square"/>
-            <c:size val="2"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="004586"/>
               </a:solidFill>
             </c:spPr>
           </c:marker>
@@ -2182,7 +2190,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$D$2:$D$10000</c:f>
+              <c:f>Sheet1!$AF$2:$AF$10000</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9999"/>
@@ -2203,11 +2211,117 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="22855719"/>
-        <c:axId val="85571983"/>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$E$1:$E$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>irr</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="004586"/>
+            </a:solidFill>
+            <a:ln w="0">
+              <a:solidFill>
+                <a:srgbClr val="004586"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="square"/>
+            <c:size val="2"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="004586"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:txPr>
+              <a:bodyPr wrap="none"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="r"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:separator> </c:separator>
+            <c:showLeaderLines val="1"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$2:$A$10000</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9999"/>
+                <c:pt idx="0">
+                  <c:v>45184</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>45185</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>45186</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>45187</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>45188</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$E$2:$E$10000</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9999"/>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:axId val="39850376"/>
+        <c:axId val="67499475"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="22855719"/>
+        <c:axId val="39850376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2253,12 +2367,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="85571983"/>
+        <c:crossAx val="67499475"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="85571983"/>
+        <c:axId val="67499475"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2295,7 +2409,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="22855719"/>
+        <c:crossAx val="39850376"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2354,9 +2468,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>432000</xdr:colOff>
+      <xdr:colOff>431640</xdr:colOff>
       <xdr:row>19</xdr:row>
-      <xdr:rowOff>121320</xdr:rowOff>
+      <xdr:rowOff>120960</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2365,7 +2479,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="330840" y="467280"/>
-        <a:ext cx="8229240" cy="2742840"/>
+        <a:ext cx="8228880" cy="2742480"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2377,16 +2491,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>10</xdr:col>
+      <xdr:col>11</xdr:col>
       <xdr:colOff>604440</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>55080</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
+      <xdr:col>21</xdr:col>
       <xdr:colOff>705600</xdr:colOff>
       <xdr:row>19</xdr:row>
-      <xdr:rowOff>34200</xdr:rowOff>
+      <xdr:rowOff>33840</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2394,8 +2508,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="8732520" y="380160"/>
-        <a:ext cx="8229240" cy="2742840"/>
+        <a:off x="9545400" y="380160"/>
+        <a:ext cx="8228880" cy="2742480"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2414,9 +2528,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>431280</xdr:colOff>
+      <xdr:colOff>430920</xdr:colOff>
       <xdr:row>38</xdr:row>
-      <xdr:rowOff>43560</xdr:rowOff>
+      <xdr:rowOff>43200</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2425,7 +2539,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="330120" y="3477960"/>
-        <a:ext cx="8229240" cy="2742840"/>
+        <a:ext cx="8228880" cy="2742480"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2437,16 +2551,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>10</xdr:col>
+      <xdr:col>11</xdr:col>
       <xdr:colOff>694080</xdr:colOff>
       <xdr:row>21</xdr:row>
       <xdr:rowOff>99000</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
+      <xdr:col>21</xdr:col>
       <xdr:colOff>795240</xdr:colOff>
       <xdr:row>38</xdr:row>
-      <xdr:rowOff>78480</xdr:rowOff>
+      <xdr:rowOff>78120</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2454,8 +2568,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="8822160" y="3512880"/>
-        <a:ext cx="8229240" cy="2742840"/>
+        <a:off x="9635040" y="3512880"/>
+        <a:ext cx="8228880" cy="2742480"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2473,7 +2587,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AF102"/>
+  <dimension ref="A1:AG102"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
@@ -2557,26 +2671,29 @@
       <c r="Y1" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="0" t="s">
+      <c r="Z1" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" s="0" t="s">
+      <c r="AA1" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" s="0" t="s">
+      <c r="AB1" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="AC1" s="0" t="s">
+      <c r="AC1" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="AD1" s="0" t="s">
+      <c r="AD1" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="AE1" s="0" t="s">
+      <c r="AE1" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="AF1" s="0" t="s">
+      <c r="AF1" s="2" t="s">
         <v>31</v>
+      </c>
+      <c r="AG1" s="2" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2589,91 +2706,94 @@
       <c r="C2" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="E2" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>32</v>
+      <c r="D2" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="F2" s="2" t="n">
+        <v>0</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="K2" s="2" t="n">
-        <v>0</v>
+        <v>33</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>33</v>
       </c>
       <c r="L2" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M2" s="2" t="s">
-        <v>32</v>
+      <c r="M2" s="2" t="n">
+        <v>0</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="O2" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="P2" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="Q2" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="R2" s="2" t="n">
-        <v>0</v>
+        <v>33</v>
+      </c>
+      <c r="R2" s="2" t="s">
+        <v>33</v>
       </c>
       <c r="S2" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="T2" s="2" t="s">
-        <v>32</v>
+      <c r="T2" s="2" t="n">
+        <v>0</v>
       </c>
       <c r="U2" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="V2" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="W2" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="X2" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="Y2" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="Z2" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="AA2" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="AB2" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="AC2" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="AD2" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="AE2" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="AF2" s="0" t="n">
+        <v>33</v>
+      </c>
+      <c r="Y2" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="Z2" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA2" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB2" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="AC2" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="AD2" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="AE2" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="AF2" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="AG2" s="2" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2688,7 +2808,7 @@
         <v>5000</v>
       </c>
       <c r="D3" s="2" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="E3" s="2" t="n">
         <v>0</v>
@@ -2696,17 +2816,17 @@
       <c r="F3" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G3" s="2" t="s">
-        <v>32</v>
+      <c r="G3" s="2" t="n">
+        <v>0</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="J3" s="2" t="n">
-        <v>0</v>
+        <v>33</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>33</v>
       </c>
       <c r="K3" s="2" t="n">
         <v>0</v>
@@ -2717,17 +2837,17 @@
       <c r="M3" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="N3" s="2" t="s">
-        <v>32</v>
+      <c r="N3" s="2" t="n">
+        <v>0</v>
       </c>
       <c r="O3" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="P3" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q3" s="2" t="n">
-        <v>0</v>
+        <v>33</v>
+      </c>
+      <c r="Q3" s="2" t="s">
+        <v>33</v>
       </c>
       <c r="R3" s="2" t="n">
         <v>0</v>
@@ -2738,40 +2858,43 @@
       <c r="T3" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U3" s="2" t="s">
-        <v>32</v>
+      <c r="U3" s="2" t="n">
+        <v>0</v>
       </c>
       <c r="V3" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="W3" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="X3" s="2" t="n">
-        <v>0</v>
+        <v>33</v>
+      </c>
+      <c r="X3" s="2" t="s">
+        <v>33</v>
       </c>
       <c r="Y3" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Z3" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="AA3" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="AB3" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="AC3" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="AD3" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="AE3" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="AF3" s="0" t="n">
+      <c r="Z3" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA3" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB3" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC3" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="AD3" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="AE3" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="AF3" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG3" s="2" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2786,7 +2909,7 @@
         <v>5000</v>
       </c>
       <c r="D4" s="2" t="n">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="E4" s="2" t="n">
         <v>0</v>
@@ -2794,17 +2917,17 @@
       <c r="F4" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G4" s="2" t="s">
-        <v>32</v>
+      <c r="G4" s="2" t="n">
+        <v>0</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="J4" s="2" t="n">
-        <v>0</v>
+        <v>33</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>33</v>
       </c>
       <c r="K4" s="2" t="n">
         <v>0</v>
@@ -2815,17 +2938,17 @@
       <c r="M4" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="N4" s="2" t="s">
-        <v>32</v>
+      <c r="N4" s="2" t="n">
+        <v>0</v>
       </c>
       <c r="O4" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="P4" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q4" s="2" t="n">
-        <v>0</v>
+        <v>33</v>
+      </c>
+      <c r="Q4" s="2" t="s">
+        <v>33</v>
       </c>
       <c r="R4" s="2" t="n">
         <v>0</v>
@@ -2836,40 +2959,43 @@
       <c r="T4" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U4" s="2" t="s">
-        <v>32</v>
+      <c r="U4" s="2" t="n">
+        <v>0</v>
       </c>
       <c r="V4" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="W4" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="X4" s="2" t="n">
-        <v>0</v>
+        <v>33</v>
+      </c>
+      <c r="X4" s="2" t="s">
+        <v>33</v>
       </c>
       <c r="Y4" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Z4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="AA4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="AB4" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="AC4" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="AD4" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="AE4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="AF4" s="0" t="n">
+      <c r="Z4" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA4" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB4" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC4" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="AD4" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="AE4" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="AF4" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG4" s="2" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2884,7 +3010,7 @@
         <v>5000</v>
       </c>
       <c r="D5" s="2" t="n">
-        <v>0</v>
+        <v>300</v>
       </c>
       <c r="E5" s="2" t="n">
         <v>0</v>
@@ -2892,17 +3018,17 @@
       <c r="F5" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G5" s="2" t="s">
-        <v>32</v>
+      <c r="G5" s="2" t="n">
+        <v>0</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="J5" s="2" t="n">
-        <v>0</v>
+        <v>33</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>33</v>
       </c>
       <c r="K5" s="2" t="n">
         <v>0</v>
@@ -2913,17 +3039,17 @@
       <c r="M5" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="N5" s="2" t="s">
-        <v>32</v>
+      <c r="N5" s="2" t="n">
+        <v>0</v>
       </c>
       <c r="O5" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="P5" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q5" s="2" t="n">
-        <v>0</v>
+        <v>33</v>
+      </c>
+      <c r="Q5" s="2" t="s">
+        <v>33</v>
       </c>
       <c r="R5" s="2" t="n">
         <v>0</v>
@@ -2934,40 +3060,43 @@
       <c r="T5" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U5" s="2" t="s">
-        <v>32</v>
+      <c r="U5" s="2" t="n">
+        <v>0</v>
       </c>
       <c r="V5" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="W5" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="X5" s="2" t="n">
-        <v>0</v>
+        <v>33</v>
+      </c>
+      <c r="X5" s="2" t="s">
+        <v>33</v>
       </c>
       <c r="Y5" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Z5" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="AA5" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="AB5" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="AC5" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="AD5" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="AE5" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="AF5" s="0" t="n">
+      <c r="Z5" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA5" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB5" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC5" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="AD5" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="AE5" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="AF5" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG5" s="2" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2982,7 +3111,7 @@
         <v>5000</v>
       </c>
       <c r="D6" s="2" t="n">
-        <v>0</v>
+        <v>400</v>
       </c>
       <c r="E6" s="2" t="n">
         <v>0</v>
@@ -2990,17 +3119,17 @@
       <c r="F6" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G6" s="2" t="s">
-        <v>32</v>
+      <c r="G6" s="2" t="n">
+        <v>0</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="J6" s="2" t="n">
-        <v>0</v>
+        <v>33</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>33</v>
       </c>
       <c r="K6" s="2" t="n">
         <v>0</v>
@@ -3011,17 +3140,17 @@
       <c r="M6" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="N6" s="2" t="s">
-        <v>32</v>
+      <c r="N6" s="2" t="n">
+        <v>0</v>
       </c>
       <c r="O6" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="P6" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q6" s="2" t="n">
-        <v>0</v>
+        <v>33</v>
+      </c>
+      <c r="Q6" s="2" t="s">
+        <v>33</v>
       </c>
       <c r="R6" s="2" t="n">
         <v>0</v>
@@ -3032,40 +3161,43 @@
       <c r="T6" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U6" s="2" t="s">
-        <v>32</v>
+      <c r="U6" s="2" t="n">
+        <v>0</v>
       </c>
       <c r="V6" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="W6" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="X6" s="2" t="n">
-        <v>0</v>
+        <v>33</v>
+      </c>
+      <c r="X6" s="2" t="s">
+        <v>33</v>
       </c>
       <c r="Y6" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Z6" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="AA6" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="AB6" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="AC6" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="AD6" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="AE6" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="AF6" s="0" t="n">
+      <c r="Z6" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA6" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB6" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC6" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="AD6" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="AE6" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="AF6" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG6" s="2" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
defaults related flow extracted
</commit_message>
<xml_diff>
--- a/stat.xlsx
+++ b/stat.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="41">
   <si>
     <t xml:space="preserve">date</t>
   </si>
@@ -77,6 +77,27 @@
   </si>
   <si>
     <t xml:space="preserve">cpy_i</t>
+  </si>
+  <si>
+    <t xml:space="preserve">revenue_d</t>
+  </si>
+  <si>
+    <t xml:space="preserve">apy1_d</t>
+  </si>
+  <si>
+    <t xml:space="preserve">apy7_d</t>
+  </si>
+  <si>
+    <t xml:space="preserve">apy30_d</t>
+  </si>
+  <si>
+    <t xml:space="preserve">apy91_d</t>
+  </si>
+  <si>
+    <t xml:space="preserve">apy_d</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cpy_d</t>
   </si>
   <si>
     <t xml:space="preserve">revenue_s</t>
@@ -245,7 +266,7 @@
       <rgbColor rgb="FFFFFF00"/>
       <rgbColor rgb="FFFF00FF"/>
       <rgbColor rgb="FF00FFFF"/>
-      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF7E0021"/>
       <rgbColor rgb="FF008000"/>
       <rgbColor rgb="FF000080"/>
       <rgbColor rgb="FF808000"/>
@@ -298,7 +319,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart108.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart21.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -462,6 +483,7 @@
                 </a:pPr>
               </a:p>
             </c:txPr>
+            <c:dLblPos val="r"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -525,11 +547,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="71426385"/>
-        <c:axId val="40110757"/>
+        <c:axId val="60580176"/>
+        <c:axId val="58084474"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="71426385"/>
+        <c:axId val="60580176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -553,7 +575,7 @@
             </a:ln>
           </c:spPr>
         </c:minorGridlines>
-        <c:numFmt formatCode="yyyy\-mm\-dd" sourceLinked="1"/>
+        <c:numFmt formatCode="yyyy\-mm\-dd" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -575,12 +597,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="40110757"/>
+        <c:crossAx val="58084474"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="40110757"/>
+        <c:axId val="58084474"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -617,7 +639,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="71426385"/>
+        <c:crossAx val="60580176"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -665,7 +687,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart109.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart22.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -680,7 +702,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$L$1:$L$1</c:f>
+              <c:f>Sheet1!$L$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -789,7 +811,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$S$1:$S$1</c:f>
+              <c:f>Sheet1!$S$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -898,11 +920,11 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$Z$1:$Z$1</c:f>
+              <c:f>Sheet1!$Z$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>cpy_s</c:v>
+                  <c:v>cpy_d</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1007,11 +1029,11 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$AG$1:$AG$1</c:f>
+              <c:f>Sheet1!$AG$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>cpy_o</c:v>
+                  <c:v>cpy_s</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1111,11 +1133,119 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="48303930"/>
-        <c:axId val="1092808"/>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$AN$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>cpy_o</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="7e0021"/>
+            </a:solidFill>
+            <a:ln w="0">
+              <a:solidFill>
+                <a:srgbClr val="7e0021"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="triangle"/>
+            <c:size val="2"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="7e0021"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:txPr>
+              <a:bodyPr wrap="none"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:separator> </c:separator>
+            <c:showLeaderLines val="1"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$2:$A$10000</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9999"/>
+                <c:pt idx="0">
+                  <c:v>45184</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>45185</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>45186</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>45187</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>45188</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$AN$2:$AN$10000</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9999"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:axId val="80799582"/>
+        <c:axId val="80929799"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="48303930"/>
+        <c:axId val="80799582"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1161,12 +1291,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1092808"/>
+        <c:crossAx val="80929799"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1092808"/>
+        <c:axId val="80929799"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1203,7 +1333,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="48303930"/>
+        <c:crossAx val="80799582"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1251,7 +1381,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart110.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart23.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1266,7 +1396,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$H$1:$H$1</c:f>
+              <c:f>Sheet1!$H$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1360,7 +1490,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$O$1:$O$1</c:f>
+              <c:f>Sheet1!$O$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1454,11 +1584,11 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$V$1:$V$1</c:f>
+              <c:f>Sheet1!$V$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>apy7_s</c:v>
+                  <c:v>apy7_d</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1548,11 +1678,11 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$AC$1:$AC$1</c:f>
+              <c:f>Sheet1!$AC$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>apy7_o</c:v>
+                  <c:v>apy7_s</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1637,11 +1767,104 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="24478412"/>
-        <c:axId val="88100120"/>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$AJ$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>apy7_o</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="7e0021"/>
+            </a:solidFill>
+            <a:ln w="0">
+              <a:solidFill>
+                <a:srgbClr val="7e0021"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="triangle"/>
+            <c:size val="2"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="7e0021"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:txPr>
+              <a:bodyPr wrap="none"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:separator> </c:separator>
+            <c:showLeaderLines val="1"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$2:$A$10000</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9999"/>
+                <c:pt idx="0">
+                  <c:v>45184</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>45185</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>45186</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>45187</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>45188</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$AJ$2:$AJ$10000</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9999"/>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:axId val="33940451"/>
+        <c:axId val="68359130"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="24478412"/>
+        <c:axId val="33940451"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1687,12 +1910,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="88100120"/>
+        <c:crossAx val="68359130"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="88100120"/>
+        <c:axId val="68359130"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1729,7 +1952,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="24478412"/>
+        <c:crossAx val="33940451"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1777,7 +2000,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart111.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart24.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1792,7 +2015,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$K$1:$K$1</c:f>
+              <c:f>Sheet1!$K$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1898,7 +2121,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$R$1:$R$1</c:f>
+              <c:f>Sheet1!$R$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2004,11 +2227,11 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$Y$1:$Y$1</c:f>
+              <c:f>Sheet1!$Y$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>apy_s</c:v>
+                  <c:v>apy_d</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2110,11 +2333,11 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$AF$1:$AF$1</c:f>
+              <c:f>Sheet1!$AF$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>apy_o</c:v>
+                  <c:v>apy_s</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2216,31 +2439,31 @@
           <c:order val="4"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$E$1:$E$1</c:f>
+              <c:f>Sheet1!$AM$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>irr</c:v>
+                  <c:v>apy_o</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:srgbClr val="004586"/>
+              <a:srgbClr val="7e0021"/>
             </a:solidFill>
             <a:ln w="0">
               <a:solidFill>
-                <a:srgbClr val="004586"/>
+                <a:srgbClr val="7e0021"/>
               </a:solidFill>
             </a:ln>
           </c:spPr>
           <c:marker>
-            <c:symbol val="square"/>
+            <c:symbol val="triangle"/>
             <c:size val="2"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="004586"/>
+                <a:srgbClr val="7e0021"/>
               </a:solidFill>
             </c:spPr>
           </c:marker>
@@ -2296,7 +2519,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$E$2:$E$10000</c:f>
+              <c:f>Sheet1!$AM$2:$AM$10000</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9999"/>
@@ -2317,11 +2540,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="39850376"/>
-        <c:axId val="67499475"/>
+        <c:axId val="82238259"/>
+        <c:axId val="48723776"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="39850376"/>
+        <c:axId val="82238259"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2367,12 +2590,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="67499475"/>
+        <c:crossAx val="48723776"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="67499475"/>
+        <c:axId val="48723776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2409,7 +2632,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="39850376"/>
+        <c:crossAx val="82238259"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2467,10 +2690,10 @@
       <xdr:rowOff>142200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>431640</xdr:colOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>214920</xdr:colOff>
       <xdr:row>19</xdr:row>
-      <xdr:rowOff>120960</xdr:rowOff>
+      <xdr:rowOff>120600</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2479,7 +2702,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="330840" y="467280"/>
-        <a:ext cx="8228880" cy="2742480"/>
+        <a:ext cx="8228520" cy="2742120"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2491,16 +2714,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>604440</xdr:colOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>25560</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>55080</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>705600</xdr:colOff>
+      <xdr:col>40</xdr:col>
+      <xdr:colOff>417960</xdr:colOff>
       <xdr:row>19</xdr:row>
-      <xdr:rowOff>33840</xdr:rowOff>
+      <xdr:rowOff>33480</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2509,7 +2732,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="9545400" y="380160"/>
-        <a:ext cx="8228880" cy="2742480"/>
+        <a:ext cx="8228520" cy="2742120"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2527,10 +2750,10 @@
       <xdr:rowOff>64080</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>430920</xdr:colOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>214200</xdr:colOff>
       <xdr:row>38</xdr:row>
-      <xdr:rowOff>43200</xdr:rowOff>
+      <xdr:rowOff>42840</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2539,7 +2762,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="330120" y="3477960"/>
-        <a:ext cx="8228880" cy="2742480"/>
+        <a:ext cx="8228520" cy="2742120"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2551,16 +2774,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>694080</xdr:colOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>115200</xdr:colOff>
       <xdr:row>21</xdr:row>
       <xdr:rowOff>99000</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>795240</xdr:colOff>
+      <xdr:col>40</xdr:col>
+      <xdr:colOff>507600</xdr:colOff>
       <xdr:row>38</xdr:row>
-      <xdr:rowOff>78120</xdr:rowOff>
+      <xdr:rowOff>77760</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2569,7 +2792,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="9635040" y="3512880"/>
-        <a:ext cx="8228880" cy="2742480"/>
+        <a:ext cx="8228520" cy="2742120"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2587,13 +2810,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AG102"/>
+  <dimension ref="A1:AN102"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="40" min="5" style="0" width="5.56"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -2695,6 +2921,27 @@
       <c r="AG1" s="2" t="s">
         <v>32</v>
       </c>
+      <c r="AH1" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="AI1" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="AJ1" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="AK1" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="AL1" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="AM1" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="AN1" s="2" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="n">
@@ -2710,25 +2957,25 @@
         <v>0</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="F2" s="2" t="n">
         <v>0</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="L2" s="2" t="n">
         <v>0</v>
@@ -2737,19 +2984,19 @@
         <v>0</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="O2" s="2" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="P2" s="2" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="Q2" s="2" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="R2" s="2" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="S2" s="2" t="n">
         <v>0</v>
@@ -2758,19 +3005,19 @@
         <v>0</v>
       </c>
       <c r="U2" s="2" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="V2" s="2" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="W2" s="2" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="X2" s="2" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="Y2" s="2" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="Z2" s="2" t="n">
         <v>0</v>
@@ -2779,21 +3026,42 @@
         <v>0</v>
       </c>
       <c r="AB2" s="2" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="AC2" s="2" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="AD2" s="2" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="AE2" s="2" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="AF2" s="2" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="AG2" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH2" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI2" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="AJ2" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="AK2" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="AL2" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="AM2" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="AN2" s="2" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2820,13 +3088,13 @@
         <v>0</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="K3" s="2" t="n">
         <v>0</v>
@@ -2841,13 +3109,13 @@
         <v>0</v>
       </c>
       <c r="O3" s="2" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="P3" s="2" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="Q3" s="2" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="R3" s="2" t="n">
         <v>0</v>
@@ -2862,13 +3130,13 @@
         <v>0</v>
       </c>
       <c r="V3" s="2" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="W3" s="2" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="X3" s="2" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="Y3" s="2" t="n">
         <v>0</v>
@@ -2883,18 +3151,39 @@
         <v>0</v>
       </c>
       <c r="AC3" s="2" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="AD3" s="2" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="AE3" s="2" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="AF3" s="2" t="n">
         <v>0</v>
       </c>
       <c r="AG3" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH3" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI3" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ3" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="AK3" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="AL3" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="AM3" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN3" s="2" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2921,13 +3210,13 @@
         <v>0</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="K4" s="2" t="n">
         <v>0</v>
@@ -2942,13 +3231,13 @@
         <v>0</v>
       </c>
       <c r="O4" s="2" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="P4" s="2" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="Q4" s="2" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="R4" s="2" t="n">
         <v>0</v>
@@ -2963,13 +3252,13 @@
         <v>0</v>
       </c>
       <c r="V4" s="2" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="W4" s="2" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="X4" s="2" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="Y4" s="2" t="n">
         <v>0</v>
@@ -2984,18 +3273,39 @@
         <v>0</v>
       </c>
       <c r="AC4" s="2" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="AD4" s="2" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="AE4" s="2" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="AF4" s="2" t="n">
         <v>0</v>
       </c>
       <c r="AG4" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH4" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI4" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ4" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="AK4" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="AL4" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="AM4" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN4" s="2" t="n">
         <v>0</v>
       </c>
     </row>
@@ -3022,13 +3332,13 @@
         <v>0</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="K5" s="2" t="n">
         <v>0</v>
@@ -3043,13 +3353,13 @@
         <v>0</v>
       </c>
       <c r="O5" s="2" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="P5" s="2" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="Q5" s="2" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="R5" s="2" t="n">
         <v>0</v>
@@ -3064,13 +3374,13 @@
         <v>0</v>
       </c>
       <c r="V5" s="2" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="W5" s="2" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="X5" s="2" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="Y5" s="2" t="n">
         <v>0</v>
@@ -3085,18 +3395,39 @@
         <v>0</v>
       </c>
       <c r="AC5" s="2" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="AD5" s="2" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="AE5" s="2" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="AF5" s="2" t="n">
         <v>0</v>
       </c>
       <c r="AG5" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH5" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI5" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ5" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="AK5" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="AL5" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="AM5" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN5" s="2" t="n">
         <v>0</v>
       </c>
     </row>
@@ -3123,13 +3454,13 @@
         <v>0</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="K6" s="2" t="n">
         <v>0</v>
@@ -3144,13 +3475,13 @@
         <v>0</v>
       </c>
       <c r="O6" s="2" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="P6" s="2" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="Q6" s="2" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="R6" s="2" t="n">
         <v>0</v>
@@ -3165,13 +3496,13 @@
         <v>0</v>
       </c>
       <c r="V6" s="2" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="W6" s="2" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="X6" s="2" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="Y6" s="2" t="n">
         <v>0</v>
@@ -3186,18 +3517,39 @@
         <v>0</v>
       </c>
       <c r="AC6" s="2" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="AD6" s="2" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="AE6" s="2" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="AF6" s="2" t="n">
         <v>0</v>
       </c>
       <c r="AG6" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH6" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI6" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ6" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="AK6" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="AL6" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="AM6" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN6" s="2" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>